<commit_message>
schema is a picture
</commit_message>
<xml_diff>
--- a/DynamoDBSQL/dynamosql/src/assets/csv/simple.xlsx
+++ b/DynamoDBSQL/dynamosql/src/assets/csv/simple.xlsx
@@ -15,6 +15,7 @@
     <sheet name="simple" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="46">
   <si>
     <t>Artist</t>
   </si>
@@ -44,34 +45,124 @@
     <t>Genre</t>
   </si>
   <si>
-    <t>Tags</t>
-  </si>
-  <si>
     <t>No One You Know</t>
   </si>
   <si>
     <t>Call Me Today</t>
   </si>
   <si>
-    <t>Somewhat Famous</t>
-  </si>
-  <si>
-    <t>{ "Composers": [ "Smith", "Jones", "Davis" ], "LengthInSeconds": 214}</t>
-  </si>
-  <si>
     <t>Call Me Tomorrow</t>
   </si>
   <si>
     <t>Country</t>
   </si>
   <si>
-    <t>{ "Composers": [ "Smith", "Jones", "Davis" ], "LengthInSeconds": 314}</t>
-  </si>
-  <si>
     <t>Don't call us, we'll call you</t>
   </si>
   <si>
-    <t>{ "Composers": [ "Smith", "Jones", "Davis" ], "LengthInSeconds": 112}</t>
+    <t>John Doe</t>
+  </si>
+  <si>
+    <t>Moscow Calling</t>
+  </si>
+  <si>
+    <t>Call Me</t>
+  </si>
+  <si>
+    <t>Blondie</t>
+  </si>
+  <si>
+    <t>The Clash</t>
+  </si>
+  <si>
+    <t>London Calling</t>
+  </si>
+  <si>
+    <t>Paul Simon</t>
+  </si>
+  <si>
+    <t>You Can Call Me Al</t>
+  </si>
+  <si>
+    <t>Carly Rae Jepsen</t>
+  </si>
+  <si>
+    <t>Call Me Maybe</t>
+  </si>
+  <si>
+    <t>The Beatles</t>
+  </si>
+  <si>
+    <t>I Call Your Name</t>
+  </si>
+  <si>
+    <t>Why didn't you call</t>
+  </si>
+  <si>
+    <t>Elton John</t>
+  </si>
+  <si>
+    <t>I Guess That's Why They Call It the Blues</t>
+  </si>
+  <si>
+    <t>The Call Up</t>
+  </si>
+  <si>
+    <t>James</t>
+  </si>
+  <si>
+    <t>Destiny Calling</t>
+  </si>
+  <si>
+    <t>A-ha</t>
+  </si>
+  <si>
+    <t>Kenny Loggins</t>
+  </si>
+  <si>
+    <t>Whenever I Call You "Friend"</t>
+  </si>
+  <si>
+    <t>Metallica</t>
+  </si>
+  <si>
+    <t>The Call of Ktulu</t>
+  </si>
+  <si>
+    <t>On Call</t>
+  </si>
+  <si>
+    <t>Last Call</t>
+  </si>
+  <si>
+    <t>This Is a Call</t>
+  </si>
+  <si>
+    <t>No One Remembers</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>Unforgettable</t>
+  </si>
+  <si>
+    <t>Forgotten</t>
+  </si>
+  <si>
+    <t>Rock</t>
+  </si>
+  <si>
+    <t>Roll</t>
+  </si>
+  <si>
+    <t>Pop</t>
+  </si>
+  <si>
+    <t>Classic</t>
+  </si>
+  <si>
+    <t>ID</t>
   </si>
 </sst>
 </file>
@@ -110,8 +201,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -392,108 +483,530 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="9.140625" style="2"/>
+    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2">
+        <f>14581</f>
+        <v>14581</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2">
-        <v>2015</v>
+      <c r="D2" t="s">
+        <v>38</v>
       </c>
       <c r="E2" s="2">
-        <v>5</v>
-      </c>
-      <c r="F2" t="s">
-        <v>10</v>
+        <v>1998</v>
+      </c>
+      <c r="F2" s="1">
+        <v>7.97</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>7</v>
+      <c r="A3">
+        <f>A2+1</f>
+        <v>14582</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
       </c>
       <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" s="2">
+        <v>2003</v>
+      </c>
+      <c r="F3" s="1">
+        <v>9.4</v>
+      </c>
+      <c r="G3" t="s">
         <v>9</v>
       </c>
-      <c r="D3">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f t="shared" ref="A4:A21" si="0">A3+1</f>
+        <v>14583</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1985</v>
+      </c>
+      <c r="F4" s="1">
+        <v>7.38</v>
+      </c>
+      <c r="G4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f t="shared" si="0"/>
+        <v>14584</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="2">
+        <v>2007</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1.97</v>
+      </c>
+      <c r="G5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f t="shared" si="0"/>
+        <v>14585</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="2">
+        <v>2016</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0.69</v>
+      </c>
+      <c r="G6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f t="shared" si="0"/>
+        <v>14586</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" s="2">
+        <v>1997</v>
+      </c>
+      <c r="F7" s="1">
+        <v>8.75</v>
+      </c>
+      <c r="G7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f t="shared" si="0"/>
+        <v>14587</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" s="2">
+        <v>1989</v>
+      </c>
+      <c r="F8" s="1">
+        <v>5.32</v>
+      </c>
+      <c r="G8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f t="shared" si="0"/>
+        <v>14588</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="2">
+        <v>2018</v>
+      </c>
+      <c r="F9" s="1">
+        <v>4.9800000000000004</v>
+      </c>
+      <c r="G9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f t="shared" si="0"/>
+        <v>14589</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" s="2">
+        <v>1985</v>
+      </c>
+      <c r="F10" s="1">
+        <v>3.99</v>
+      </c>
+      <c r="G10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f t="shared" si="0"/>
+        <v>14590</v>
+      </c>
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" t="str">
+        <f>"Random "&amp;B11&amp;" Album"</f>
+        <v>Random Blondie Album</v>
+      </c>
+      <c r="E11" s="2">
+        <v>1984</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="G11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f t="shared" si="0"/>
+        <v>14591</v>
+      </c>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" ref="D12:D21" si="1">"Random "&amp;B12&amp;" Album"</f>
+        <v>Random The Clash Album</v>
+      </c>
+      <c r="E12" s="2">
         <v>2015</v>
       </c>
-      <c r="E3">
-        <v>3</v>
-      </c>
-      <c r="F3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4">
+      <c r="F12" s="1">
+        <v>8.7100000000000009</v>
+      </c>
+      <c r="G12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f t="shared" si="0"/>
+        <v>14592</v>
+      </c>
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="1"/>
+        <v>Random Paul Simon Album</v>
+      </c>
+      <c r="E13" s="2">
+        <v>2013</v>
+      </c>
+      <c r="F13" s="1">
+        <v>7.3</v>
+      </c>
+      <c r="G13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f t="shared" si="0"/>
+        <v>14593</v>
+      </c>
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="1"/>
+        <v>Random Carly Rae Jepsen Album</v>
+      </c>
+      <c r="E14" s="2">
+        <v>1998</v>
+      </c>
+      <c r="F14" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="G14" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f t="shared" si="0"/>
+        <v>14594</v>
+      </c>
+      <c r="B15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="1"/>
+        <v>Random The Beatles Album</v>
+      </c>
+      <c r="E15" s="2">
+        <v>2007</v>
+      </c>
+      <c r="F15" s="1">
+        <v>6.38</v>
+      </c>
+      <c r="G15" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <f t="shared" si="0"/>
+        <v>14595</v>
+      </c>
+      <c r="B16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="1"/>
+        <v>Random Elton John Album</v>
+      </c>
+      <c r="E16" s="2">
+        <v>2016</v>
+      </c>
+      <c r="F16" s="1">
+        <v>7.08</v>
+      </c>
+      <c r="G16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f t="shared" si="0"/>
+        <v>14596</v>
+      </c>
+      <c r="B17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" si="1"/>
+        <v>Random The Clash Album</v>
+      </c>
+      <c r="E17" s="2">
+        <v>2016</v>
+      </c>
+      <c r="F17" s="1">
+        <v>0.17</v>
+      </c>
+      <c r="G17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <f t="shared" si="0"/>
+        <v>14597</v>
+      </c>
+      <c r="B18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="1"/>
+        <v>Random James Album</v>
+      </c>
+      <c r="E18" s="2">
+        <v>1971</v>
+      </c>
+      <c r="F18" s="1">
+        <v>8.9600000000000009</v>
+      </c>
+      <c r="G18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <f t="shared" si="0"/>
+        <v>14598</v>
+      </c>
+      <c r="B19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" si="1"/>
+        <v>Random A-ha Album</v>
+      </c>
+      <c r="E19" s="2">
+        <v>2003</v>
+      </c>
+      <c r="F19" s="1">
+        <v>3.73</v>
+      </c>
+      <c r="G19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <f t="shared" si="0"/>
+        <v>14599</v>
+      </c>
+      <c r="B20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" t="s">
+        <v>31</v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" si="1"/>
+        <v>Random Kenny Loggins Album</v>
+      </c>
+      <c r="E20" s="2">
+        <v>1995</v>
+      </c>
+      <c r="F20" s="1">
+        <v>4.17</v>
+      </c>
+      <c r="G20" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <f t="shared" si="0"/>
+        <v>14600</v>
+      </c>
+      <c r="B21" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" t="str">
+        <f t="shared" si="1"/>
+        <v>Random Metallica Album</v>
+      </c>
+      <c r="E21" s="2">
         <v>2015</v>
       </c>
-      <c r="E4">
-        <v>4</v>
-      </c>
-      <c r="F4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
+      <c r="F21" s="1">
+        <v>7.71</v>
+      </c>
+      <c r="G21" t="s">
+        <v>43</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
UNION support is added
</commit_message>
<xml_diff>
--- a/DynamoDBSQL/dynamosql/src/assets/csv/simple.xlsx
+++ b/DynamoDBSQL/dynamosql/src/assets/csv/simple.xlsx
@@ -25,25 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="46">
-  <si>
-    <t>Artist</t>
-  </si>
-  <si>
-    <t>SongTitle</t>
-  </si>
-  <si>
-    <t>AlbumTitle</t>
-  </si>
-  <si>
-    <t>Year</t>
-  </si>
-  <si>
-    <t>Price</t>
-  </si>
-  <si>
-    <t>Genre</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="46">
   <si>
     <t>No One You Know</t>
   </si>
@@ -162,7 +144,25 @@
     <t>Classic</t>
   </si>
   <si>
-    <t>ID</t>
+    <t>id</t>
+  </si>
+  <si>
+    <t>artist</t>
+  </si>
+  <si>
+    <t>album</t>
+  </si>
+  <si>
+    <t>song</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>genre</t>
   </si>
 </sst>
 </file>
@@ -486,7 +486,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -499,25 +499,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1" t="s">
         <v>45</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -526,19 +526,22 @@
         <v>14581</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="E2" s="2">
         <v>1998</v>
       </c>
       <c r="F2" s="1">
         <v>7.97</v>
+      </c>
+      <c r="G2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -547,13 +550,13 @@
         <v>14582</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="E3" s="2">
         <v>2003</v>
@@ -562,7 +565,7 @@
         <v>9.4</v>
       </c>
       <c r="G3" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -571,13 +574,13 @@
         <v>14583</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="E4" s="2">
         <v>1985</v>
@@ -586,7 +589,7 @@
         <v>7.38</v>
       </c>
       <c r="G4" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -595,13 +598,13 @@
         <v>14584</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="E5" s="2">
         <v>2007</v>
@@ -610,7 +613,7 @@
         <v>1.97</v>
       </c>
       <c r="G5" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -619,13 +622,13 @@
         <v>14585</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="E6" s="2">
         <v>2016</v>
@@ -634,7 +637,7 @@
         <v>0.69</v>
       </c>
       <c r="G6" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -643,13 +646,13 @@
         <v>14586</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D7" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="E7" s="2">
         <v>1997</v>
@@ -658,7 +661,7 @@
         <v>8.75</v>
       </c>
       <c r="G7" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -667,13 +670,13 @@
         <v>14587</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D8" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="E8" s="2">
         <v>1989</v>
@@ -682,7 +685,7 @@
         <v>5.32</v>
       </c>
       <c r="G8" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -691,13 +694,13 @@
         <v>14588</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D9" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="E9" s="2">
         <v>2018</v>
@@ -706,7 +709,7 @@
         <v>4.9800000000000004</v>
       </c>
       <c r="G9" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -715,13 +718,13 @@
         <v>14589</v>
       </c>
       <c r="B10" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C10" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D10" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="E10" s="2">
         <v>1985</v>
@@ -730,7 +733,7 @@
         <v>3.99</v>
       </c>
       <c r="G10" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -739,10 +742,10 @@
         <v>14590</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D11" t="str">
         <f>"Random "&amp;B11&amp;" Album"</f>
@@ -755,7 +758,7 @@
         <v>0.01</v>
       </c>
       <c r="G11" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -764,10 +767,10 @@
         <v>14591</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D12" t="str">
         <f t="shared" ref="D12:D21" si="1">"Random "&amp;B12&amp;" Album"</f>
@@ -780,7 +783,7 @@
         <v>8.7100000000000009</v>
       </c>
       <c r="G12" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -789,10 +792,10 @@
         <v>14592</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D13" t="str">
         <f t="shared" si="1"/>
@@ -805,7 +808,7 @@
         <v>7.3</v>
       </c>
       <c r="G13" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -814,10 +817,10 @@
         <v>14593</v>
       </c>
       <c r="B14" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D14" t="str">
         <f t="shared" si="1"/>
@@ -830,7 +833,7 @@
         <v>1.5</v>
       </c>
       <c r="G14" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -839,10 +842,10 @@
         <v>14594</v>
       </c>
       <c r="B15" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C15" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D15" t="str">
         <f t="shared" si="1"/>
@@ -855,7 +858,7 @@
         <v>6.38</v>
       </c>
       <c r="G15" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -864,10 +867,10 @@
         <v>14595</v>
       </c>
       <c r="B16" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C16" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D16" t="str">
         <f t="shared" si="1"/>
@@ -880,7 +883,7 @@
         <v>7.08</v>
       </c>
       <c r="G16" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -889,10 +892,10 @@
         <v>14596</v>
       </c>
       <c r="B17" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C17" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D17" t="str">
         <f t="shared" si="1"/>
@@ -905,7 +908,7 @@
         <v>0.17</v>
       </c>
       <c r="G17" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -914,10 +917,10 @@
         <v>14597</v>
       </c>
       <c r="B18" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C18" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D18" t="str">
         <f t="shared" si="1"/>
@@ -930,7 +933,7 @@
         <v>8.9600000000000009</v>
       </c>
       <c r="G18" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -939,10 +942,10 @@
         <v>14598</v>
       </c>
       <c r="B19" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C19" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D19" t="str">
         <f t="shared" si="1"/>
@@ -955,7 +958,7 @@
         <v>3.73</v>
       </c>
       <c r="G19" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -964,10 +967,10 @@
         <v>14599</v>
       </c>
       <c r="B20" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C20" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D20" t="str">
         <f t="shared" si="1"/>
@@ -980,7 +983,7 @@
         <v>4.17</v>
       </c>
       <c r="G20" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -989,10 +992,10 @@
         <v>14600</v>
       </c>
       <c r="B21" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C21" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D21" t="str">
         <f t="shared" si="1"/>
@@ -1005,7 +1008,7 @@
         <v>7.71</v>
       </c>
       <c r="G21" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
First task works. Several runs implemented.
</commit_message>
<xml_diff>
--- a/DynamoDBSQL/dynamosql/src/assets/csv/simple.xlsx
+++ b/DynamoDBSQL/dynamosql/src/assets/csv/simple.xlsx
@@ -13,9 +13,9 @@
   </bookViews>
   <sheets>
     <sheet name="simple" sheetId="1" r:id="rId1"/>
+    <sheet name="CLI_generation" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="48">
   <si>
     <t>No One You Know</t>
   </si>
@@ -163,6 +163,12 @@
   </si>
   <si>
     <t>genre</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>S</t>
   </si>
 </sst>
 </file>
@@ -486,7 +492,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -538,7 +544,7 @@
         <v>1998</v>
       </c>
       <c r="F2" s="1">
-        <v>7.97</v>
+        <v>1.5</v>
       </c>
       <c r="G2" t="s">
         <v>3</v>
@@ -562,7 +568,7 @@
         <v>2003</v>
       </c>
       <c r="F3" s="1">
-        <v>9.4</v>
+        <v>0.25</v>
       </c>
       <c r="G3" t="s">
         <v>3</v>
@@ -586,7 +592,7 @@
         <v>1985</v>
       </c>
       <c r="F4" s="1">
-        <v>7.38</v>
+        <v>2</v>
       </c>
       <c r="G4" t="s">
         <v>3</v>
@@ -610,7 +616,7 @@
         <v>2007</v>
       </c>
       <c r="F5" s="1">
-        <v>1.97</v>
+        <v>1</v>
       </c>
       <c r="G5" t="s">
         <v>32</v>
@@ -634,7 +640,7 @@
         <v>2016</v>
       </c>
       <c r="F6" s="1">
-        <v>0.69</v>
+        <v>0.5</v>
       </c>
       <c r="G6" t="s">
         <v>35</v>
@@ -658,7 +664,7 @@
         <v>1997</v>
       </c>
       <c r="F7" s="1">
-        <v>8.75</v>
+        <v>0.5</v>
       </c>
       <c r="G7" t="s">
         <v>36</v>
@@ -682,7 +688,7 @@
         <v>1989</v>
       </c>
       <c r="F8" s="1">
-        <v>5.32</v>
+        <v>0.5</v>
       </c>
       <c r="G8" t="s">
         <v>38</v>
@@ -706,7 +712,7 @@
         <v>2018</v>
       </c>
       <c r="F9" s="1">
-        <v>4.9800000000000004</v>
+        <v>1.25</v>
       </c>
       <c r="G9" t="s">
         <v>35</v>
@@ -1015,4 +1021,1116 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3:F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <f>14581</f>
+        <v>14581</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1998</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="G3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" t="str">
+        <f>""""&amp;A$1&amp;""""&amp;": { """&amp;A$2&amp;""":"&amp;""""&amp;A3&amp;"""},"</f>
+        <v>"id": { "N":"14581"},</v>
+      </c>
+      <c r="I3" t="str">
+        <f t="shared" ref="I3:N3" si="0">""""&amp;B$1&amp;""""&amp;": { """&amp;B$2&amp;""":"&amp;""""&amp;B3&amp;"""},"</f>
+        <v>"artist": { "S":"John Doe"},</v>
+      </c>
+      <c r="J3" t="str">
+        <f t="shared" si="0"/>
+        <v>"song": { "S":"Call Me Today"},</v>
+      </c>
+      <c r="K3" t="str">
+        <f t="shared" si="0"/>
+        <v>"album": { "S":"Unknown"},</v>
+      </c>
+      <c r="L3" t="str">
+        <f t="shared" si="0"/>
+        <v>"year": { "N":"1998"},</v>
+      </c>
+      <c r="M3" t="str">
+        <f t="shared" si="0"/>
+        <v>"price": { "N":"1,5"},</v>
+      </c>
+      <c r="N3" t="str">
+        <f t="shared" si="0"/>
+        <v>"genre": { "S":"Country"},</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f>A3+1</f>
+        <v>14582</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1998</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="G4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H4" t="str">
+        <f t="shared" ref="H4:H22" si="1">""""&amp;A$1&amp;""""&amp;": { """&amp;A$2&amp;""":"&amp;""""&amp;A4&amp;"""},"</f>
+        <v>"id": { "N":"14582"},</v>
+      </c>
+      <c r="I4" t="str">
+        <f t="shared" ref="I4:I22" si="2">""""&amp;B$1&amp;""""&amp;": { """&amp;B$2&amp;""":"&amp;""""&amp;B4&amp;"""},"</f>
+        <v>"artist": { "S":"John Doe"},</v>
+      </c>
+      <c r="J4" t="str">
+        <f t="shared" ref="J4:J22" si="3">""""&amp;C$1&amp;""""&amp;": { """&amp;C$2&amp;""":"&amp;""""&amp;C4&amp;"""},"</f>
+        <v>"song": { "S":"Call Me Tomorrow"},</v>
+      </c>
+      <c r="K4" t="str">
+        <f t="shared" ref="K4:K22" si="4">""""&amp;D$1&amp;""""&amp;": { """&amp;D$2&amp;""":"&amp;""""&amp;D4&amp;"""},"</f>
+        <v>"album": { "S":"Unknown"},</v>
+      </c>
+      <c r="L4" t="str">
+        <f t="shared" ref="L4:L22" si="5">""""&amp;E$1&amp;""""&amp;": { """&amp;E$2&amp;""":"&amp;""""&amp;E4&amp;"""},"</f>
+        <v>"year": { "N":"1998"},</v>
+      </c>
+      <c r="M4" t="str">
+        <f t="shared" ref="M4:M22" si="6">""""&amp;F$1&amp;""""&amp;": { """&amp;F$2&amp;""":"&amp;""""&amp;F4&amp;"""},"</f>
+        <v>"price": { "N":"0,25"},</v>
+      </c>
+      <c r="N4" t="str">
+        <f t="shared" ref="N4:N22" si="7">""""&amp;G$1&amp;""""&amp;": { """&amp;G$2&amp;""":"&amp;""""&amp;G4&amp;"""},"</f>
+        <v>"genre": { "S":"Country"},</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f t="shared" ref="A5:A22" si="8">A4+1</f>
+        <v>14583</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="2">
+        <v>1998</v>
+      </c>
+      <c r="F5" s="1">
+        <v>2</v>
+      </c>
+      <c r="G5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H5" t="str">
+        <f t="shared" si="1"/>
+        <v>"id": { "N":"14583"},</v>
+      </c>
+      <c r="I5" t="str">
+        <f t="shared" si="2"/>
+        <v>"artist": { "S":"John Doe"},</v>
+      </c>
+      <c r="J5" t="str">
+        <f t="shared" si="3"/>
+        <v>"song": { "S":"Don't call us, we'll call you"},</v>
+      </c>
+      <c r="K5" t="str">
+        <f t="shared" si="4"/>
+        <v>"album": { "S":"Unknown"},</v>
+      </c>
+      <c r="L5" t="str">
+        <f t="shared" si="5"/>
+        <v>"year": { "N":"1998"},</v>
+      </c>
+      <c r="M5" t="str">
+        <f t="shared" si="6"/>
+        <v>"price": { "N":"2"},</v>
+      </c>
+      <c r="N5" t="str">
+        <f t="shared" si="7"/>
+        <v>"genre": { "S":"Country"},</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f t="shared" si="8"/>
+        <v>14584</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="2">
+        <v>1998</v>
+      </c>
+      <c r="F6" s="1">
+        <v>1</v>
+      </c>
+      <c r="G6" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6" t="str">
+        <f t="shared" si="1"/>
+        <v>"id": { "N":"14584"},</v>
+      </c>
+      <c r="I6" t="str">
+        <f t="shared" si="2"/>
+        <v>"artist": { "S":"John Doe"},</v>
+      </c>
+      <c r="J6" t="str">
+        <f t="shared" si="3"/>
+        <v>"song": { "S":"Moscow Calling"},</v>
+      </c>
+      <c r="K6" t="str">
+        <f t="shared" si="4"/>
+        <v>"album": { "S":"Unknown"},</v>
+      </c>
+      <c r="L6" t="str">
+        <f t="shared" si="5"/>
+        <v>"year": { "N":"1998"},</v>
+      </c>
+      <c r="M6" t="str">
+        <f t="shared" si="6"/>
+        <v>"price": { "N":"1"},</v>
+      </c>
+      <c r="N6" t="str">
+        <f t="shared" si="7"/>
+        <v>"genre": { "S":"Unknown"},</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f t="shared" si="8"/>
+        <v>14585</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="2">
+        <v>1998</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="G7" t="s">
+        <v>35</v>
+      </c>
+      <c r="H7" t="str">
+        <f t="shared" si="1"/>
+        <v>"id": { "N":"14585"},</v>
+      </c>
+      <c r="I7" t="str">
+        <f t="shared" si="2"/>
+        <v>"artist": { "S":"John Doe"},</v>
+      </c>
+      <c r="J7" t="str">
+        <f t="shared" si="3"/>
+        <v>"song": { "S":"Why didn't you call"},</v>
+      </c>
+      <c r="K7" t="str">
+        <f t="shared" si="4"/>
+        <v>"album": { "S":"Unknown"},</v>
+      </c>
+      <c r="L7" t="str">
+        <f t="shared" si="5"/>
+        <v>"year": { "N":"1998"},</v>
+      </c>
+      <c r="M7" t="str">
+        <f t="shared" si="6"/>
+        <v>"price": { "N":"0,1"},</v>
+      </c>
+      <c r="N7" t="str">
+        <f t="shared" si="7"/>
+        <v>"genre": { "S":"Rock"},</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f t="shared" si="8"/>
+        <v>14586</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="2">
+        <v>1998</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="G8" t="s">
+        <v>36</v>
+      </c>
+      <c r="H8" t="str">
+        <f t="shared" si="1"/>
+        <v>"id": { "N":"14586"},</v>
+      </c>
+      <c r="I8" t="str">
+        <f t="shared" si="2"/>
+        <v>"artist": { "S":"John Doe"},</v>
+      </c>
+      <c r="J8" t="str">
+        <f t="shared" si="3"/>
+        <v>"song": { "S":"On Call"},</v>
+      </c>
+      <c r="K8" t="str">
+        <f t="shared" si="4"/>
+        <v>"album": { "S":"Unknown"},</v>
+      </c>
+      <c r="L8" t="str">
+        <f t="shared" si="5"/>
+        <v>"year": { "N":"1998"},</v>
+      </c>
+      <c r="M8" t="str">
+        <f t="shared" si="6"/>
+        <v>"price": { "N":"0,1"},</v>
+      </c>
+      <c r="N8" t="str">
+        <f t="shared" si="7"/>
+        <v>"genre": { "S":"Roll"},</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f t="shared" si="8"/>
+        <v>14587</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="2">
+        <v>1998</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="G9" t="s">
+        <v>38</v>
+      </c>
+      <c r="H9" t="str">
+        <f t="shared" si="1"/>
+        <v>"id": { "N":"14587"},</v>
+      </c>
+      <c r="I9" t="str">
+        <f t="shared" si="2"/>
+        <v>"artist": { "S":"John Doe"},</v>
+      </c>
+      <c r="J9" t="str">
+        <f t="shared" si="3"/>
+        <v>"song": { "S":"Last Call"},</v>
+      </c>
+      <c r="K9" t="str">
+        <f t="shared" si="4"/>
+        <v>"album": { "S":"Unknown"},</v>
+      </c>
+      <c r="L9" t="str">
+        <f t="shared" si="5"/>
+        <v>"year": { "N":"1998"},</v>
+      </c>
+      <c r="M9" t="str">
+        <f t="shared" si="6"/>
+        <v>"price": { "N":"0,1"},</v>
+      </c>
+      <c r="N9" t="str">
+        <f t="shared" si="7"/>
+        <v>"genre": { "S":"Classic"},</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f t="shared" si="8"/>
+        <v>14588</v>
+      </c>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="2">
+        <v>1998</v>
+      </c>
+      <c r="F10" s="1">
+        <v>1.25</v>
+      </c>
+      <c r="G10" t="s">
+        <v>35</v>
+      </c>
+      <c r="H10" t="str">
+        <f t="shared" si="1"/>
+        <v>"id": { "N":"14588"},</v>
+      </c>
+      <c r="I10" t="str">
+        <f t="shared" si="2"/>
+        <v>"artist": { "S":"John Doe"},</v>
+      </c>
+      <c r="J10" t="str">
+        <f t="shared" si="3"/>
+        <v>"song": { "S":"This Is a Call"},</v>
+      </c>
+      <c r="K10" t="str">
+        <f t="shared" si="4"/>
+        <v>"album": { "S":"Unknown"},</v>
+      </c>
+      <c r="L10" t="str">
+        <f t="shared" si="5"/>
+        <v>"year": { "N":"1998"},</v>
+      </c>
+      <c r="M10" t="str">
+        <f t="shared" si="6"/>
+        <v>"price": { "N":"1,25"},</v>
+      </c>
+      <c r="N10" t="str">
+        <f t="shared" si="7"/>
+        <v>"genre": { "S":"Rock"},</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f t="shared" si="8"/>
+        <v>14589</v>
+      </c>
+      <c r="B11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="2">
+        <v>1985</v>
+      </c>
+      <c r="F11" s="1">
+        <v>3.99</v>
+      </c>
+      <c r="G11" t="s">
+        <v>34</v>
+      </c>
+      <c r="H11" t="str">
+        <f t="shared" si="1"/>
+        <v>"id": { "N":"14589"},</v>
+      </c>
+      <c r="I11" t="str">
+        <f t="shared" si="2"/>
+        <v>"artist": { "S":"No One You Know"},</v>
+      </c>
+      <c r="J11" t="str">
+        <f t="shared" si="3"/>
+        <v>"song": { "S":"No One Remembers"},</v>
+      </c>
+      <c r="K11" t="str">
+        <f t="shared" si="4"/>
+        <v>"album": { "S":"Unforgettable"},</v>
+      </c>
+      <c r="L11" t="str">
+        <f t="shared" si="5"/>
+        <v>"year": { "N":"1985"},</v>
+      </c>
+      <c r="M11" t="str">
+        <f t="shared" si="6"/>
+        <v>"price": { "N":"3,99"},</v>
+      </c>
+      <c r="N11" t="str">
+        <f t="shared" si="7"/>
+        <v>"genre": { "S":"Forgotten"},</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f t="shared" si="8"/>
+        <v>14590</v>
+      </c>
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" t="str">
+        <f>"Random "&amp;B12&amp;" Album"</f>
+        <v>Random Blondie Album</v>
+      </c>
+      <c r="E12" s="2">
+        <v>1984</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="G12" t="s">
+        <v>37</v>
+      </c>
+      <c r="H12" t="str">
+        <f t="shared" si="1"/>
+        <v>"id": { "N":"14590"},</v>
+      </c>
+      <c r="I12" t="str">
+        <f t="shared" si="2"/>
+        <v>"artist": { "S":"Blondie"},</v>
+      </c>
+      <c r="J12" t="str">
+        <f t="shared" si="3"/>
+        <v>"song": { "S":"Call Me"},</v>
+      </c>
+      <c r="K12" t="str">
+        <f t="shared" si="4"/>
+        <v>"album": { "S":"Random Blondie Album"},</v>
+      </c>
+      <c r="L12" t="str">
+        <f t="shared" si="5"/>
+        <v>"year": { "N":"1984"},</v>
+      </c>
+      <c r="M12" t="str">
+        <f t="shared" si="6"/>
+        <v>"price": { "N":"0,01"},</v>
+      </c>
+      <c r="N12" t="str">
+        <f t="shared" si="7"/>
+        <v>"genre": { "S":"Pop"},</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f t="shared" si="8"/>
+        <v>14591</v>
+      </c>
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" ref="D13:D22" si="9">"Random "&amp;B13&amp;" Album"</f>
+        <v>Random The Clash Album</v>
+      </c>
+      <c r="E13" s="2">
+        <v>2015</v>
+      </c>
+      <c r="F13" s="1">
+        <v>8.7100000000000009</v>
+      </c>
+      <c r="G13" t="s">
+        <v>37</v>
+      </c>
+      <c r="H13" t="str">
+        <f t="shared" si="1"/>
+        <v>"id": { "N":"14591"},</v>
+      </c>
+      <c r="I13" t="str">
+        <f t="shared" si="2"/>
+        <v>"artist": { "S":"The Clash"},</v>
+      </c>
+      <c r="J13" t="str">
+        <f t="shared" si="3"/>
+        <v>"song": { "S":"London Calling"},</v>
+      </c>
+      <c r="K13" t="str">
+        <f t="shared" si="4"/>
+        <v>"album": { "S":"Random The Clash Album"},</v>
+      </c>
+      <c r="L13" t="str">
+        <f t="shared" si="5"/>
+        <v>"year": { "N":"2015"},</v>
+      </c>
+      <c r="M13" t="str">
+        <f t="shared" si="6"/>
+        <v>"price": { "N":"8,71"},</v>
+      </c>
+      <c r="N13" t="str">
+        <f t="shared" si="7"/>
+        <v>"genre": { "S":"Pop"},</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f t="shared" si="8"/>
+        <v>14592</v>
+      </c>
+      <c r="B14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="9"/>
+        <v>Random Paul Simon Album</v>
+      </c>
+      <c r="E14" s="2">
+        <v>2013</v>
+      </c>
+      <c r="F14" s="1">
+        <v>7.3</v>
+      </c>
+      <c r="G14" t="s">
+        <v>37</v>
+      </c>
+      <c r="H14" t="str">
+        <f t="shared" si="1"/>
+        <v>"id": { "N":"14592"},</v>
+      </c>
+      <c r="I14" t="str">
+        <f t="shared" si="2"/>
+        <v>"artist": { "S":"Paul Simon"},</v>
+      </c>
+      <c r="J14" t="str">
+        <f t="shared" si="3"/>
+        <v>"song": { "S":"You Can Call Me Al"},</v>
+      </c>
+      <c r="K14" t="str">
+        <f t="shared" si="4"/>
+        <v>"album": { "S":"Random Paul Simon Album"},</v>
+      </c>
+      <c r="L14" t="str">
+        <f t="shared" si="5"/>
+        <v>"year": { "N":"2013"},</v>
+      </c>
+      <c r="M14" t="str">
+        <f t="shared" si="6"/>
+        <v>"price": { "N":"7,3"},</v>
+      </c>
+      <c r="N14" t="str">
+        <f t="shared" si="7"/>
+        <v>"genre": { "S":"Pop"},</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f t="shared" si="8"/>
+        <v>14593</v>
+      </c>
+      <c r="B15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="9"/>
+        <v>Random Carly Rae Jepsen Album</v>
+      </c>
+      <c r="E15" s="2">
+        <v>1998</v>
+      </c>
+      <c r="F15" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="G15" t="s">
+        <v>37</v>
+      </c>
+      <c r="H15" t="str">
+        <f t="shared" si="1"/>
+        <v>"id": { "N":"14593"},</v>
+      </c>
+      <c r="I15" t="str">
+        <f t="shared" si="2"/>
+        <v>"artist": { "S":"Carly Rae Jepsen"},</v>
+      </c>
+      <c r="J15" t="str">
+        <f t="shared" si="3"/>
+        <v>"song": { "S":"Call Me Maybe"},</v>
+      </c>
+      <c r="K15" t="str">
+        <f t="shared" si="4"/>
+        <v>"album": { "S":"Random Carly Rae Jepsen Album"},</v>
+      </c>
+      <c r="L15" t="str">
+        <f t="shared" si="5"/>
+        <v>"year": { "N":"1998"},</v>
+      </c>
+      <c r="M15" t="str">
+        <f t="shared" si="6"/>
+        <v>"price": { "N":"1,5"},</v>
+      </c>
+      <c r="N15" t="str">
+        <f t="shared" si="7"/>
+        <v>"genre": { "S":"Pop"},</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <f t="shared" si="8"/>
+        <v>14594</v>
+      </c>
+      <c r="B16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="9"/>
+        <v>Random The Beatles Album</v>
+      </c>
+      <c r="E16" s="2">
+        <v>2007</v>
+      </c>
+      <c r="F16" s="1">
+        <v>6.38</v>
+      </c>
+      <c r="G16" t="s">
+        <v>37</v>
+      </c>
+      <c r="H16" t="str">
+        <f t="shared" si="1"/>
+        <v>"id": { "N":"14594"},</v>
+      </c>
+      <c r="I16" t="str">
+        <f t="shared" si="2"/>
+        <v>"artist": { "S":"The Beatles"},</v>
+      </c>
+      <c r="J16" t="str">
+        <f t="shared" si="3"/>
+        <v>"song": { "S":"I Call Your Name"},</v>
+      </c>
+      <c r="K16" t="str">
+        <f t="shared" si="4"/>
+        <v>"album": { "S":"Random The Beatles Album"},</v>
+      </c>
+      <c r="L16" t="str">
+        <f t="shared" si="5"/>
+        <v>"year": { "N":"2007"},</v>
+      </c>
+      <c r="M16" t="str">
+        <f t="shared" si="6"/>
+        <v>"price": { "N":"6,38"},</v>
+      </c>
+      <c r="N16" t="str">
+        <f t="shared" si="7"/>
+        <v>"genre": { "S":"Pop"},</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f t="shared" si="8"/>
+        <v>14595</v>
+      </c>
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" si="9"/>
+        <v>Random Elton John Album</v>
+      </c>
+      <c r="E17" s="2">
+        <v>2016</v>
+      </c>
+      <c r="F17" s="1">
+        <v>7.08</v>
+      </c>
+      <c r="G17" t="s">
+        <v>37</v>
+      </c>
+      <c r="H17" t="str">
+        <f t="shared" si="1"/>
+        <v>"id": { "N":"14595"},</v>
+      </c>
+      <c r="I17" t="str">
+        <f t="shared" si="2"/>
+        <v>"artist": { "S":"Elton John"},</v>
+      </c>
+      <c r="J17" t="str">
+        <f t="shared" si="3"/>
+        <v>"song": { "S":"I Guess That's Why They Call It the Blues"},</v>
+      </c>
+      <c r="K17" t="str">
+        <f t="shared" si="4"/>
+        <v>"album": { "S":"Random Elton John Album"},</v>
+      </c>
+      <c r="L17" t="str">
+        <f t="shared" si="5"/>
+        <v>"year": { "N":"2016"},</v>
+      </c>
+      <c r="M17" t="str">
+        <f t="shared" si="6"/>
+        <v>"price": { "N":"7,08"},</v>
+      </c>
+      <c r="N17" t="str">
+        <f t="shared" si="7"/>
+        <v>"genre": { "S":"Pop"},</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <f t="shared" si="8"/>
+        <v>14596</v>
+      </c>
+      <c r="B18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" t="s">
+        <v>20</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="9"/>
+        <v>Random The Clash Album</v>
+      </c>
+      <c r="E18" s="2">
+        <v>2016</v>
+      </c>
+      <c r="F18" s="1">
+        <v>0.17</v>
+      </c>
+      <c r="G18" t="s">
+        <v>37</v>
+      </c>
+      <c r="H18" t="str">
+        <f t="shared" si="1"/>
+        <v>"id": { "N":"14596"},</v>
+      </c>
+      <c r="I18" t="str">
+        <f t="shared" si="2"/>
+        <v>"artist": { "S":"The Clash"},</v>
+      </c>
+      <c r="J18" t="str">
+        <f t="shared" si="3"/>
+        <v>"song": { "S":"The Call Up"},</v>
+      </c>
+      <c r="K18" t="str">
+        <f t="shared" si="4"/>
+        <v>"album": { "S":"Random The Clash Album"},</v>
+      </c>
+      <c r="L18" t="str">
+        <f t="shared" si="5"/>
+        <v>"year": { "N":"2016"},</v>
+      </c>
+      <c r="M18" t="str">
+        <f t="shared" si="6"/>
+        <v>"price": { "N":"0,17"},</v>
+      </c>
+      <c r="N18" t="str">
+        <f t="shared" si="7"/>
+        <v>"genre": { "S":"Pop"},</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <f t="shared" si="8"/>
+        <v>14597</v>
+      </c>
+      <c r="B19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" si="9"/>
+        <v>Random James Album</v>
+      </c>
+      <c r="E19" s="2">
+        <v>1971</v>
+      </c>
+      <c r="F19" s="1">
+        <v>8.9600000000000009</v>
+      </c>
+      <c r="G19" t="s">
+        <v>37</v>
+      </c>
+      <c r="H19" t="str">
+        <f t="shared" si="1"/>
+        <v>"id": { "N":"14597"},</v>
+      </c>
+      <c r="I19" t="str">
+        <f t="shared" si="2"/>
+        <v>"artist": { "S":"James"},</v>
+      </c>
+      <c r="J19" t="str">
+        <f t="shared" si="3"/>
+        <v>"song": { "S":"Destiny Calling"},</v>
+      </c>
+      <c r="K19" t="str">
+        <f t="shared" si="4"/>
+        <v>"album": { "S":"Random James Album"},</v>
+      </c>
+      <c r="L19" t="str">
+        <f t="shared" si="5"/>
+        <v>"year": { "N":"1971"},</v>
+      </c>
+      <c r="M19" t="str">
+        <f t="shared" si="6"/>
+        <v>"price": { "N":"8,96"},</v>
+      </c>
+      <c r="N19" t="str">
+        <f t="shared" si="7"/>
+        <v>"genre": { "S":"Pop"},</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <f t="shared" si="8"/>
+        <v>14598</v>
+      </c>
+      <c r="B20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" si="9"/>
+        <v>Random A-ha Album</v>
+      </c>
+      <c r="E20" s="2">
+        <v>2003</v>
+      </c>
+      <c r="F20" s="1">
+        <v>3.73</v>
+      </c>
+      <c r="G20" t="s">
+        <v>37</v>
+      </c>
+      <c r="H20" t="str">
+        <f t="shared" si="1"/>
+        <v>"id": { "N":"14598"},</v>
+      </c>
+      <c r="I20" t="str">
+        <f t="shared" si="2"/>
+        <v>"artist": { "S":"A-ha"},</v>
+      </c>
+      <c r="J20" t="str">
+        <f t="shared" si="3"/>
+        <v>"song": { "S":"I Call Your Name"},</v>
+      </c>
+      <c r="K20" t="str">
+        <f t="shared" si="4"/>
+        <v>"album": { "S":"Random A-ha Album"},</v>
+      </c>
+      <c r="L20" t="str">
+        <f t="shared" si="5"/>
+        <v>"year": { "N":"2003"},</v>
+      </c>
+      <c r="M20" t="str">
+        <f t="shared" si="6"/>
+        <v>"price": { "N":"3,73"},</v>
+      </c>
+      <c r="N20" t="str">
+        <f t="shared" si="7"/>
+        <v>"genre": { "S":"Pop"},</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <f t="shared" si="8"/>
+        <v>14599</v>
+      </c>
+      <c r="B21" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" t="str">
+        <f t="shared" si="9"/>
+        <v>Random Kenny Loggins Album</v>
+      </c>
+      <c r="E21" s="2">
+        <v>1995</v>
+      </c>
+      <c r="F21" s="1">
+        <v>4.17</v>
+      </c>
+      <c r="G21" t="s">
+        <v>37</v>
+      </c>
+      <c r="H21" t="str">
+        <f t="shared" si="1"/>
+        <v>"id": { "N":"14599"},</v>
+      </c>
+      <c r="I21" t="str">
+        <f t="shared" si="2"/>
+        <v>"artist": { "S":"Kenny Loggins"},</v>
+      </c>
+      <c r="J21" t="str">
+        <f t="shared" si="3"/>
+        <v>"song": { "S":"Whenever I Call You "Friend""},</v>
+      </c>
+      <c r="K21" t="str">
+        <f t="shared" si="4"/>
+        <v>"album": { "S":"Random Kenny Loggins Album"},</v>
+      </c>
+      <c r="L21" t="str">
+        <f t="shared" si="5"/>
+        <v>"year": { "N":"1995"},</v>
+      </c>
+      <c r="M21" t="str">
+        <f t="shared" si="6"/>
+        <v>"price": { "N":"4,17"},</v>
+      </c>
+      <c r="N21" t="str">
+        <f t="shared" si="7"/>
+        <v>"genre": { "S":"Pop"},</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <f t="shared" si="8"/>
+        <v>14600</v>
+      </c>
+      <c r="B22" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" t="str">
+        <f t="shared" si="9"/>
+        <v>Random Metallica Album</v>
+      </c>
+      <c r="E22" s="2">
+        <v>2015</v>
+      </c>
+      <c r="F22" s="1">
+        <v>7.71</v>
+      </c>
+      <c r="G22" t="s">
+        <v>37</v>
+      </c>
+      <c r="H22" t="str">
+        <f t="shared" si="1"/>
+        <v>"id": { "N":"14600"},</v>
+      </c>
+      <c r="I22" t="str">
+        <f t="shared" si="2"/>
+        <v>"artist": { "S":"Metallica"},</v>
+      </c>
+      <c r="J22" t="str">
+        <f t="shared" si="3"/>
+        <v>"song": { "S":"The Call of Ktulu"},</v>
+      </c>
+      <c r="K22" t="str">
+        <f t="shared" si="4"/>
+        <v>"album": { "S":"Random Metallica Album"},</v>
+      </c>
+      <c r="L22" t="str">
+        <f t="shared" si="5"/>
+        <v>"year": { "N":"2015"},</v>
+      </c>
+      <c r="M22" t="str">
+        <f t="shared" si="6"/>
+        <v>"price": { "N":"7,71"},</v>
+      </c>
+      <c r="N22" t="str">
+        <f t="shared" si="7"/>
+        <v>"genre": { "S":"Pop"},</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>